<commit_message>
added courses and labs for software engineering
</commit_message>
<xml_diff>
--- a/Anul 3/Semestrul 1/Inginerie Software/Laborator/Lab 4 Sprint Capacity Model.xlsx
+++ b/Anul 3/Semestrul 1/Inginerie Software/Laborator/Lab 4 Sprint Capacity Model.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26124"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_75484E46551D2A31FB88BD72DA79C1252EA92133" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C59FAAF5-7A54-4D96-9042-A786B598C518}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="11_75484E46551D2A31FB88BD72DA79C1252EA92133" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D6BB360-3B07-42FA-9DC4-B4965E843A21}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>Sprint Capacity Planner</t>
   </si>
@@ -105,25 +105,13 @@
     <t>Sprint Length (Days)</t>
   </si>
   <si>
-    <t>Jarca Andrei</t>
-  </si>
-  <si>
     <t>Hours per day</t>
-  </si>
-  <si>
-    <t>Ioana V.</t>
   </si>
   <si>
     <t>Focus Factor</t>
   </si>
   <si>
-    <t>Popel Bogdan</t>
-  </si>
-  <si>
     <t>Daily stand-ups (Hours/Sprint)</t>
-  </si>
-  <si>
-    <t>Diana Cristiana</t>
   </si>
   <si>
     <t>Sprint Planning Duration (Hours/Sprint)</t>
@@ -1136,7 +1124,7 @@
   <dimension ref="B1:S1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1229,7 +1217,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="60">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E5" s="60"/>
       <c r="F5" s="56"/>
@@ -1281,25 +1269,23 @@
       </c>
       <c r="E6" s="60"/>
       <c r="F6" s="52"/>
-      <c r="G6" s="62" t="s">
-        <v>8</v>
-      </c>
+      <c r="G6" s="62"/>
       <c r="H6" s="63">
         <v>1</v>
       </c>
       <c r="I6" s="64">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
+      <c r="K6" s="64">
+        <v>1.5</v>
+      </c>
       <c r="L6" s="64">
         <v>2</v>
       </c>
-      <c r="M6" s="64">
-        <v>4</v>
-      </c>
+      <c r="M6" s="64"/>
       <c r="N6" s="64">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O6" s="64"/>
       <c r="P6" s="64"/>
@@ -1314,115 +1300,87 @@
     <row r="7" spans="2:19" ht="14.25" customHeight="1">
       <c r="B7" s="4"/>
       <c r="C7" s="59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="60">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E7" s="60"/>
       <c r="F7" s="52"/>
-      <c r="G7" s="65" t="s">
-        <v>10</v>
-      </c>
+      <c r="G7" s="65"/>
       <c r="H7" s="66">
         <v>1</v>
       </c>
       <c r="I7" s="67">
-        <f t="shared" ref="I7:J7" si="0">$D$7*$H$7</f>
         <v>1.5</v>
       </c>
       <c r="J7" s="67">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K7" s="67">
         <v>1.5</v>
       </c>
       <c r="L7" s="67">
-        <f t="shared" ref="L7:N7" si="1">$D$7*$H$7</f>
-        <v>1.5</v>
-      </c>
-      <c r="M7" s="67">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M7" s="67"/>
       <c r="N7" s="67">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="O7" s="67">
-        <v>1.5</v>
-      </c>
-      <c r="P7" s="67">
-        <f t="shared" ref="P7:R7" si="2">$D$7*$H$7</f>
-        <v>1.5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
       <c r="Q7" s="67">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="R7" s="67">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="S7" s="3"/>
     </row>
     <row r="8" spans="2:19" ht="14.25" customHeight="1">
       <c r="B8" s="4"/>
       <c r="C8" s="59" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" s="68">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="69"/>
       <c r="F8" s="52"/>
-      <c r="G8" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="G8" s="62"/>
       <c r="H8" s="63">
         <v>1</v>
       </c>
       <c r="I8" s="64">
-        <f t="shared" ref="I8:J8" si="3">$D$7*$H$8</f>
         <v>1.5</v>
       </c>
-      <c r="J8" s="64">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
+      <c r="J8" s="64"/>
       <c r="K8" s="64"/>
       <c r="L8" s="64">
-        <f t="shared" ref="L8:N8" si="4">$D$7*$H$8</f>
-        <v>1.5</v>
-      </c>
-      <c r="M8" s="64">
-        <f t="shared" si="4"/>
-        <v>1.5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M8" s="64"/>
       <c r="N8" s="64">
-        <f t="shared" si="4"/>
-        <v>1.5</v>
-      </c>
-      <c r="O8" s="64"/>
+        <v>2</v>
+      </c>
+      <c r="O8" s="64">
+        <v>2</v>
+      </c>
       <c r="P8" s="64">
-        <f t="shared" ref="P8:R8" si="5">$D$7*$H$8</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="64">
-        <f t="shared" si="5"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="R8" s="64">
-        <f t="shared" si="5"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="2:19" ht="14.25" customHeight="1">
       <c r="B9" s="4"/>
       <c r="C9" s="59" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D9" s="70">
         <f>0.25</f>
@@ -1430,81 +1388,88 @@
       </c>
       <c r="E9" s="69">
         <f>D5*D9*D6</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F9" s="52"/>
-      <c r="G9" s="65" t="s">
-        <v>14</v>
-      </c>
+      <c r="G9" s="65"/>
       <c r="H9" s="66">
         <v>1</v>
       </c>
       <c r="I9" s="67">
+        <v>1.5</v>
+      </c>
+      <c r="J9" s="67">
         <v>2</v>
-      </c>
-      <c r="J9" s="67">
-        <f>$D$7*$H$9</f>
-        <v>1.5</v>
       </c>
       <c r="K9" s="67"/>
       <c r="L9" s="67">
-        <f t="shared" ref="L9:N9" si="6">$D$7*$H$9</f>
-        <v>1.5</v>
-      </c>
-      <c r="M9" s="67">
-        <f t="shared" si="6"/>
-        <v>1.5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M9" s="67"/>
       <c r="N9" s="67">
-        <f t="shared" si="6"/>
-        <v>1.5</v>
-      </c>
-      <c r="O9" s="67"/>
+        <v>2</v>
+      </c>
+      <c r="O9" s="67">
+        <v>2</v>
+      </c>
       <c r="P9" s="67">
-        <f t="shared" ref="P9:R9" si="7">$D$7*$H$9</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="Q9" s="67">
-        <f t="shared" si="7"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="R9" s="67">
-        <f t="shared" si="7"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="2:19" ht="14.25" customHeight="1">
       <c r="B10" s="4"/>
       <c r="C10" s="59" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D10" s="69">
         <v>1.5</v>
       </c>
       <c r="E10" s="69">
         <f>D5*D10</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F10" s="52"/>
       <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64"/>
+      <c r="H10" s="63">
+        <v>1</v>
+      </c>
+      <c r="I10" s="64">
+        <v>1.5</v>
+      </c>
       <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
+      <c r="K10" s="64">
+        <v>1.5</v>
+      </c>
+      <c r="L10" s="64">
+        <v>2</v>
+      </c>
       <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
+      <c r="N10" s="64">
+        <v>2</v>
+      </c>
+      <c r="O10" s="64">
+        <v>2</v>
+      </c>
+      <c r="P10" s="64">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="64">
+        <v>2</v>
+      </c>
+      <c r="R10" s="8"/>
       <c r="S10" s="3"/>
     </row>
     <row r="11" spans="2:19" ht="14.25" customHeight="1">
       <c r="B11" s="4"/>
       <c r="C11" s="59" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D11" s="70">
         <f>20/60</f>
@@ -1512,34 +1477,52 @@
       </c>
       <c r="E11" s="70">
         <f>D5*D11</f>
-        <v>1.3333333333333333</v>
+        <v>2</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="65"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
+      <c r="H11" s="66">
+        <v>1</v>
+      </c>
+      <c r="I11" s="67">
+        <v>1.5</v>
+      </c>
+      <c r="J11" s="67">
+        <v>1</v>
+      </c>
+      <c r="K11" s="67">
+        <v>1.5</v>
+      </c>
+      <c r="L11" s="67">
+        <v>2</v>
+      </c>
       <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
+      <c r="N11" s="67">
+        <v>2</v>
+      </c>
+      <c r="O11" s="67">
+        <v>2</v>
+      </c>
       <c r="P11" s="67"/>
-      <c r="Q11" s="67"/>
-      <c r="R11" s="67"/>
+      <c r="Q11" s="67">
+        <v>2</v>
+      </c>
+      <c r="R11" s="67">
+        <v>2</v>
+      </c>
       <c r="S11" s="3"/>
     </row>
     <row r="12" spans="2:19" ht="14.25" customHeight="1">
       <c r="B12" s="4"/>
       <c r="C12" s="59" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D12" s="69">
         <v>0.5</v>
       </c>
       <c r="E12" s="69">
         <f>D5*D12</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="52"/>
       <c r="G12" s="62"/>
@@ -1559,14 +1542,14 @@
     <row r="13" spans="2:19" ht="14.25" customHeight="1">
       <c r="B13" s="4"/>
       <c r="C13" s="59" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D13" s="69">
         <v>1.5</v>
       </c>
       <c r="E13" s="69">
         <f>D5*D13</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F13" s="52"/>
       <c r="G13" s="65"/>
@@ -1586,14 +1569,14 @@
     <row r="14" spans="2:19" ht="14.25" customHeight="1">
       <c r="B14" s="4"/>
       <c r="C14" s="59" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D14" s="69">
         <v>0.5</v>
       </c>
       <c r="E14" s="69">
         <f>D5*D14</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="52"/>
       <c r="G14" s="62"/>
@@ -1633,11 +1616,11 @@
     <row r="16" spans="2:19" ht="14.25" customHeight="1">
       <c r="B16" s="4"/>
       <c r="C16" s="72" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D16" s="73">
         <f>R17</f>
-        <v>55.5</v>
+        <v>80</v>
       </c>
       <c r="E16" s="53"/>
       <c r="F16" s="52"/>
@@ -1658,16 +1641,16 @@
     <row r="17" spans="2:19" ht="14.25" customHeight="1">
       <c r="B17" s="4"/>
       <c r="C17" s="72" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D17" s="74">
         <f>SUM(E9:E14)</f>
-        <v>27.333333333333332</v>
+        <v>41</v>
       </c>
       <c r="E17" s="53"/>
       <c r="F17" s="52"/>
       <c r="G17" s="80" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H17" s="87"/>
       <c r="I17" s="87"/>
@@ -1681,18 +1664,18 @@
       <c r="Q17" s="87"/>
       <c r="R17" s="81">
         <f>SUM(I6:R14)</f>
-        <v>55.5</v>
+        <v>80</v>
       </c>
       <c r="S17" s="3"/>
     </row>
     <row r="18" spans="2:19" ht="14.25" customHeight="1">
       <c r="B18" s="4"/>
       <c r="C18" s="72" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D18" s="75">
         <f>(D16-D17)*(1-D8)</f>
-        <v>4.2250000000000005</v>
+        <v>19.5</v>
       </c>
       <c r="E18" s="53"/>
       <c r="F18" s="52"/>
@@ -1713,11 +1696,11 @@
     <row r="19" spans="2:19" ht="14.25" customHeight="1">
       <c r="B19" s="4"/>
       <c r="C19" s="72" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D19" s="76">
         <f>(D16-D17)*D8</f>
-        <v>23.941666666666666</v>
+        <v>19.5</v>
       </c>
       <c r="E19" s="60"/>
       <c r="F19" s="52"/>
@@ -1738,11 +1721,11 @@
     <row r="20" spans="2:19" ht="14.25" customHeight="1">
       <c r="B20" s="4"/>
       <c r="C20" s="72" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D20" s="77">
         <f>D19/8</f>
-        <v>2.9927083333333333</v>
+        <v>2.4375</v>
       </c>
       <c r="E20" s="60"/>
       <c r="F20" s="52"/>
@@ -2779,7 +2762,7 @@
     <mergeCell ref="G17:Q18"/>
     <mergeCell ref="R17:R18"/>
   </mergeCells>
-  <conditionalFormatting sqref="H6:R15">
+  <conditionalFormatting sqref="H6:R9 H11:R15 H10:Q10">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2895,7 +2878,7 @@
       <c r="E4" s="22"/>
       <c r="F4" s="17"/>
       <c r="G4" s="23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>6</v>
@@ -2944,7 +2927,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="24"/>
       <c r="G5" s="25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H5" s="26">
         <v>1</v>
@@ -2985,7 +2968,7 @@
       <c r="A6" s="9"/>
       <c r="B6" s="13"/>
       <c r="C6" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="22">
         <v>8</v>
@@ -2993,7 +2976,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="24"/>
       <c r="G6" s="28" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H6" s="29">
         <v>1</v>
@@ -3034,7 +3017,7 @@
       <c r="A7" s="9"/>
       <c r="B7" s="13"/>
       <c r="C7" s="21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="31">
         <v>0.8</v>
@@ -3042,7 +3025,7 @@
       <c r="E7" s="32"/>
       <c r="F7" s="24"/>
       <c r="G7" s="25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H7" s="26">
         <v>1</v>
@@ -3083,7 +3066,7 @@
       <c r="A8" s="9"/>
       <c r="B8" s="13"/>
       <c r="C8" s="21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" s="32">
         <v>0.25</v>
@@ -3093,7 +3076,7 @@
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H8" s="29">
         <v>0.75</v>
@@ -3134,7 +3117,7 @@
       <c r="A9" s="9"/>
       <c r="B9" s="13"/>
       <c r="C9" s="21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D9" s="32">
         <v>4.5</v>
@@ -3144,7 +3127,7 @@
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H9" s="26">
         <v>0.5</v>
@@ -3185,7 +3168,7 @@
       <c r="A10" s="9"/>
       <c r="B10" s="13"/>
       <c r="C10" s="21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10" s="32">
         <v>2</v>
@@ -3195,7 +3178,7 @@
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H10" s="34"/>
       <c r="I10" s="34">
@@ -3255,7 +3238,7 @@
       <c r="A12" s="9"/>
       <c r="B12" s="13"/>
       <c r="C12" s="35" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D12" s="36">
         <v>334</v>
@@ -3280,7 +3263,7 @@
       <c r="A13" s="9"/>
       <c r="B13" s="13"/>
       <c r="C13" s="35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D13" s="36">
         <v>45</v>
@@ -3288,7 +3271,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="24"/>
       <c r="G13" s="84" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H13" s="89"/>
       <c r="I13" s="89"/>
@@ -3309,7 +3292,7 @@
       <c r="A14" s="9"/>
       <c r="B14" s="13"/>
       <c r="C14" s="35" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D14" s="37">
         <v>57.8</v>
@@ -3334,7 +3317,7 @@
       <c r="A15" s="9"/>
       <c r="B15" s="13"/>
       <c r="C15" s="35" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D15" s="38">
         <v>231</v>
@@ -24030,25 +24013,25 @@
   <sheetData>
     <row r="1" spans="2:16">
       <c r="B1" s="91" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" s="89"/>
       <c r="D1" s="89"/>
       <c r="E1" s="89"/>
       <c r="F1" s="91" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G1" s="89"/>
       <c r="H1" s="89"/>
       <c r="I1" s="89"/>
       <c r="J1" s="91" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K1" s="89"/>
       <c r="L1" s="89"/>
       <c r="M1" s="89"/>
       <c r="N1" s="44" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="2:16">
@@ -24102,31 +24085,31 @@
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
       <c r="I3" s="92" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J3" s="93"/>
       <c r="K3" s="92" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L3" s="93"/>
       <c r="M3" s="92" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="N3" s="93"/>
       <c r="O3" s="92" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="P3" s="93"/>
     </row>
     <row r="4" spans="2:16">
       <c r="B4" s="94" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" s="89"/>
     </row>
     <row r="5" spans="2:16">
       <c r="C5" s="95" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
@@ -24134,18 +24117,18 @@
     </row>
     <row r="6" spans="2:16">
       <c r="G6" s="96" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H6" s="89"/>
     </row>
     <row r="7" spans="2:16">
       <c r="I7" s="45" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:16">
       <c r="I8" s="46" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:16">
@@ -24153,7 +24136,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="47" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K9" s="47">
         <v>4</v>
@@ -24164,7 +24147,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K10" s="47">
         <v>3</v>
@@ -24175,7 +24158,7 @@
         <v>3</v>
       </c>
       <c r="J11" s="47" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K11" s="47">
         <v>2</v>
@@ -24183,7 +24166,7 @@
     </row>
     <row r="12" spans="2:16">
       <c r="J12" s="97" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K12" s="89"/>
     </row>
@@ -24192,7 +24175,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="47" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K13" s="47"/>
       <c r="L13" s="47"/>
@@ -24206,7 +24189,7 @@
         <v>5</v>
       </c>
       <c r="J14" s="44" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="M14" s="44">
         <v>5</v>
@@ -24217,7 +24200,7 @@
         <v>6</v>
       </c>
       <c r="J15" s="47" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K15" s="47"/>
       <c r="L15" s="47"/>
@@ -24231,7 +24214,7 @@
         <v>7</v>
       </c>
       <c r="J16" s="44" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M16" s="44">
         <v>4</v>
@@ -24239,7 +24222,7 @@
     </row>
     <row r="17" spans="1:26">
       <c r="A17" s="91" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B17" s="89"/>
       <c r="C17" s="89"/>
@@ -24269,7 +24252,7 @@
     </row>
     <row r="18" spans="1:26">
       <c r="I18" s="48" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:26">
@@ -24277,7 +24260,7 @@
         <v>8</v>
       </c>
       <c r="J19" s="47" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K19" s="47"/>
       <c r="L19" s="47"/>
@@ -24291,7 +24274,7 @@
         <v>9</v>
       </c>
       <c r="J20" s="47" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K20" s="47"/>
       <c r="L20" s="47"/>
@@ -24305,7 +24288,7 @@
         <v>10</v>
       </c>
       <c r="J21" s="47" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K21" s="47"/>
       <c r="L21" s="47"/>
@@ -24316,33 +24299,28 @@
     </row>
     <row r="22" spans="1:26">
       <c r="L22" s="49" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M22" s="49"/>
       <c r="N22" s="49"/>
     </row>
     <row r="23" spans="1:26">
       <c r="M23" s="49" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:26">
       <c r="I24" s="50" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:26">
       <c r="P26" s="45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="A17:Z17"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
@@ -24350,6 +24328,11 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A17:Z17"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <legacyDrawing r:id="rId1"/>
@@ -24370,16 +24353,16 @@
     <row r="1" spans="1:26">
       <c r="I1" s="44"/>
       <c r="J1" s="44" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L1" s="44" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N1" s="44" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P1" s="44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -24387,7 +24370,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="47" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="Q2" s="47"/>
     </row>
@@ -24396,7 +24379,7 @@
         <v>2</v>
       </c>
       <c r="P3" s="47" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="Q3" s="47"/>
     </row>
@@ -24405,7 +24388,7 @@
         <v>3</v>
       </c>
       <c r="P4" s="47" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="Q4" s="47"/>
     </row>
@@ -24424,7 +24407,7 @@
     </row>
     <row r="7" spans="1:26">
       <c r="P7" s="47" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -24435,12 +24418,12 @@
       <c r="L8" s="47"/>
       <c r="M8" s="47"/>
       <c r="N8" s="47" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="91" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B10" s="89"/>
       <c r="C10" s="89"/>
@@ -24480,7 +24463,7 @@
       <c r="M12" s="47"/>
       <c r="N12" s="44"/>
       <c r="P12" s="47" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -24492,7 +24475,7 @@
       <c r="M13" s="47"/>
       <c r="N13" s="44"/>
       <c r="P13" s="47" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -24504,7 +24487,7 @@
       <c r="M14" s="47"/>
       <c r="N14" s="44"/>
       <c r="P14" s="47" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -24517,23 +24500,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DF1F5BF9BA03CD448733D401D2715B86" ma:contentTypeVersion="6" ma:contentTypeDescription="Creați un document nou." ma:contentTypeScope="" ma:versionID="de7b10b0ebe57482c947b57b5b73fb39">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d040b213-39be-4216-a7d7-4c420e05192f" xmlns:ns3="d5984b22-f06d-428a-9753-d5eac3e5b778" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f02af7d96bbbc09070aa954fa4bf278b" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DF1F5BF9BA03CD448733D401D2715B86" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c319908db5fd00f991a64bc1845f090">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d040b213-39be-4216-a7d7-4c420e05192f" xmlns:ns3="d5984b22-f06d-428a-9753-d5eac3e5b778" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b231174e851e0aa6135f59a7a0b5a9a5" ns2:_="" ns3:_="">
     <xsd:import namespace="d040b213-39be-4216-a7d7-4c420e05192f"/>
     <xsd:import namespace="d5984b22-f06d-428a-9753-d5eac3e5b778"/>
     <xsd:element name="properties">
@@ -24548,6 +24516,11 @@
                 <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -24558,7 +24531,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d040b213-39be-4216-a7d7-4c420e05192f" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Partajat cu" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -24577,12 +24550,23 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Partajat cu detalii" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{d9aee7e1-18f7-45f4-99b2-baa0db6433f8}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d040b213-39be-4216-a7d7-4c420e05192f">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d5984b22-f06d-428a-9753-d5eac3e5b778" elementFormDefault="qualified">
@@ -24608,6 +24592,30 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="f5cd9f51-4d1e-4d57-bf3d-f118fc5c8090" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
@@ -24618,8 +24626,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tip de conținut"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titlu"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -24708,8 +24716,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5984b22-f06d-428a-9753-d5eac3e5b778">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d040b213-39be-4216-a7d7-4c420e05192f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA2E356-37A2-4326-814F-D3B7C6AD2B3E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D645D97-AE19-4A12-9067-E9D3F981A8C0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24717,5 +24745,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2678C070-115C-43C8-84AB-2CD237593F8E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA2E356-37A2-4326-814F-D3B7C6AD2B3E}"/>
 </file>
</xml_diff>